<commit_message>
rm useless invariant d4297f267ddc606a440c7977fdd9f936b31e44c3
</commit_message>
<xml_diff>
--- a/ig/nr-update-annuaire-dependency/StructureDefinition-PDSmintendedrecipient.xlsx
+++ b/ig/nr-update-annuaire-dependency/StructureDefinition-PDSmintendedrecipient.xlsx
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-11T09:02:59+00:00</t>
+    <t>2023-07-26T14:54:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>